<commit_message>
Enable plain api actions.
</commit_message>
<xml_diff>
--- a/meta/api/SampleMethodTest.xlsx
+++ b/meta/api/SampleMethodTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9078DC16-64BD-E542-8019-2F8CEE77DF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD6ECB1-D223-114A-B89B-F966236B7F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="641" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="641" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -4262,8 +4262,8 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7574,7 +7574,7 @@
   </sheetPr>
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:D14"/>
     </sheetView>
   </sheetViews>
@@ -8612,6 +8612,8 @@
     <mergeCell ref="F42:F43"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B30:G30"/>
     <mergeCell ref="N42:O42"/>
     <mergeCell ref="P42:Q42"/>
     <mergeCell ref="S42:S43"/>
@@ -8621,8 +8623,6 @@
     <mergeCell ref="J42:J43"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="L42:L43"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="B30:G30"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B38:G38"/>
@@ -12938,7 +12938,7 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>